<commit_message>
重构Action及ActionManager，框架完成; 功能只完成了queue parallel start end 和 moveby; IDE换成vscode;
</commit_message>
<xml_diff>
--- a/api list.xlsx
+++ b/api list.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="3105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="4305" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="402">
   <si>
     <t>精灵类</t>
   </si>
@@ -1052,12 +1052,432 @@
   <si>
     <t>是否激活（设为默认消息层），默认为true</t>
   </si>
+  <si>
+    <t>storefont</t>
+  </si>
+  <si>
+    <t>暂存字体信息</t>
+  </si>
+  <si>
+    <t>如果多次storefont，只会保存最后一次的结果。用restorefont命令可以将字体设为最后一次storefont时的状态。</t>
+  </si>
+  <si>
+    <t>restorefont</t>
+  </si>
+  <si>
+    <t>复原字体信息</t>
+  </si>
+  <si>
+    <t>动作</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>queue</t>
+  </si>
+  <si>
+    <t>创建一个命令队列，用于按顺序执行命令</t>
+  </si>
+  <si>
+    <t>parallel</t>
+  </si>
+  <si>
+    <t>创建一个并行命令集合，用于同时执行命令。结束时间按照最长的动作时间计算。</t>
+  </si>
+  <si>
+    <t>moveby</t>
+  </si>
+  <si>
+    <t>*pos</t>
+  </si>
+  <si>
+    <t>相对移动的坐标</t>
+  </si>
+  <si>
+    <t>控制精灵相对移动的动作</t>
+  </si>
+  <si>
+    <t>time==0</t>
+  </si>
+  <si>
+    <t>动作的持续时间，默认为0</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>动作的目标</t>
+  </si>
+  <si>
+    <t>ease</t>
+  </si>
+  <si>
+    <t>字符串 string / 数型 number</t>
+  </si>
+  <si>
+    <t>动作的速率变化（详情见说明）</t>
+  </si>
+  <si>
+    <t>moveto</t>
+  </si>
+  <si>
+    <t>绝对移动的坐标</t>
+  </si>
+  <si>
+    <t>控制精灵绝对移动的动作</t>
+  </si>
+  <si>
+    <t>fadeto</t>
+  </si>
+  <si>
+    <t>*opacity</t>
+  </si>
+  <si>
+    <t>将要渐变到的目标透明度</t>
+  </si>
+  <si>
+    <t>控制精灵透明度渐变的动作</t>
+  </si>
+  <si>
+    <t>scaleby</t>
+  </si>
+  <si>
+    <t>动作持续的时间，默认为0</t>
+  </si>
+  <si>
+    <t>控制精灵相对缩放某一倍数的动作</t>
+  </si>
+  <si>
+    <t>x=100</t>
+  </si>
+  <si>
+    <t>百分比型 percent_t</t>
+  </si>
+  <si>
+    <t>x上的缩放倍数，默认为100</t>
+  </si>
+  <si>
+    <t>y=100</t>
+  </si>
+  <si>
+    <t>y上的缩放倍数，默认为100</t>
+  </si>
+  <si>
+    <t>scaleto</t>
+  </si>
+  <si>
+    <t>控制精灵绝对缩放到某一倍数的动作</t>
+  </si>
+  <si>
+    <t>rotateby</t>
+  </si>
+  <si>
+    <t>*rotate</t>
+  </si>
+  <si>
+    <t>将旋转至的角度</t>
+  </si>
+  <si>
+    <t>控制精灵相对旋转某一角度的动作</t>
+  </si>
+  <si>
+    <t>rotateto</t>
+  </si>
+  <si>
+    <t>将旋转的角度</t>
+  </si>
+  <si>
+    <t>控制精灵绝对旋转至某一角度的动作</t>
+  </si>
+  <si>
+    <t>tintby</t>
+  </si>
+  <si>
+    <t>*r</t>
+  </si>
+  <si>
+    <t>将要变至的色调（红色部分）</t>
+  </si>
+  <si>
+    <t>控制精灵色调改变某一颜色的动作</t>
+  </si>
+  <si>
+    <t>*g</t>
+  </si>
+  <si>
+    <t>将要变至的色调（绿色部分）</t>
+  </si>
+  <si>
+    <t>*b</t>
+  </si>
+  <si>
+    <t>将要变至的色调（蓝色部分）</t>
+  </si>
+  <si>
+    <t>tintto</t>
+  </si>
+  <si>
+    <t>*color</t>
+  </si>
+  <si>
+    <t>将要变至的色调</t>
+  </si>
+  <si>
+    <t>控制精灵色调变至某一颜色的动作</t>
+  </si>
+  <si>
+    <t>jump</t>
+  </si>
+  <si>
+    <t>动作的持续的时间（单次）</t>
+  </si>
+  <si>
+    <t>精灵执行向上跳动的动作</t>
+  </si>
+  <si>
+    <t>跳动的幅度（正向上，负向下）</t>
+  </si>
+  <si>
+    <t>x=0</t>
+  </si>
+  <si>
+    <t>水平位移，默认为0</t>
+  </si>
+  <si>
+    <t>times</t>
+  </si>
+  <si>
+    <t>动作执行的次数（若为负数，则动作无限重复）</t>
+  </si>
+  <si>
+    <t>shake</t>
+  </si>
+  <si>
+    <t>动作的持续时间（单次）</t>
+  </si>
+  <si>
+    <t>精灵执行摇动的动作</t>
+  </si>
+  <si>
+    <t>*range</t>
+  </si>
+  <si>
+    <t>摇动的范围</t>
+  </si>
+  <si>
+    <t>vertical=false</t>
+  </si>
+  <si>
+    <t>是否是上下摇动（默认false）</t>
+  </si>
+  <si>
+    <t>quake</t>
+  </si>
+  <si>
+    <t>震动</t>
+  </si>
+  <si>
+    <t>rangex=0</t>
+  </si>
+  <si>
+    <t>横向摇动的范围，默认为0</t>
+  </si>
+  <si>
+    <t>rangey=0</t>
+  </si>
+  <si>
+    <t>纵向摇动的范围，默认为0</t>
+  </si>
+  <si>
+    <t>speed=1000</t>
+  </si>
+  <si>
+    <t>每秒震动的最大次数</t>
+  </si>
+  <si>
+    <t>visible</t>
+  </si>
+  <si>
+    <t>*visible</t>
+  </si>
+  <si>
+    <t>是否可见</t>
+  </si>
+  <si>
+    <t>调整精灵是否可见</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>是否销毁该精灵</t>
+  </si>
+  <si>
+    <t>从该精灵的父精灵上移除它</t>
+  </si>
+  <si>
+    <t>flipx</t>
+  </si>
+  <si>
+    <t>force=false</t>
+  </si>
+  <si>
+    <t>是否连同所有子精灵一起翻转，默认为false</t>
+  </si>
+  <si>
+    <t>水平翻转</t>
+  </si>
+  <si>
+    <t>flipy</t>
+  </si>
+  <si>
+    <t>垂直翻转</t>
+  </si>
+  <si>
+    <t>scissorby</t>
+  </si>
+  <si>
+    <t>*rect</t>
+  </si>
+  <si>
+    <t>将要改变的范围</t>
+  </si>
+  <si>
+    <t>相对改变某个精灵显示图像的范围</t>
+  </si>
+  <si>
+    <t>scissorto</t>
+  </si>
+  <si>
+    <t>绝对改变某个精灵显示图像的范围</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>延迟的时间</t>
+  </si>
+  <si>
+    <t>只能用于queue或者parallel中，用于两个动作间的时间间隔</t>
+  </si>
+  <si>
+    <t>callback</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>标签</t>
+  </si>
+  <si>
+    <t>只能用于queue或者parallel中，用于某个时间点访问指定脚本</t>
+  </si>
+  <si>
+    <t>文件，默认为当前文件</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>执行的表达式</t>
+  </si>
+  <si>
+    <t>param</t>
+  </si>
+  <si>
+    <t>字典型 dictionary</t>
+  </si>
+  <si>
+    <t>参数</t>
+  </si>
+  <si>
+    <t>wait=true</t>
+  </si>
+  <si>
+    <t>是否等待callback完成才继续动作（默认true）</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>haky3d</t>
+    </r>
+  </si>
+  <si>
+    <t>动作的持续时间</t>
+  </si>
+  <si>
+    <t>网格的震动效果</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>num=10</t>
+    </r>
+  </si>
+  <si>
+    <t>横向网格数</t>
+  </si>
+  <si>
+    <t>vnum=10</t>
+  </si>
+  <si>
+    <t>纵向网格数</t>
+  </si>
+  <si>
+    <t>offset=5</t>
+  </si>
+  <si>
+    <t>震动的偏移量</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>队列的目标</t>
+  </si>
+  <si>
+    <t>只能用于queue或者parallel中，结束当前queue或者parallel创建并添加到上一级queue或者parallel最后。若没有上一级，则什么都不做。</t>
+  </si>
+  <si>
+    <t>队列重复执行的次数，负数表示一直执行下去，默认为1</t>
+  </si>
+  <si>
+    <t>若在创建queue或parallel的过程中，立刻结束所有层动作的创建（相当于执行若干个end），并立刻开始创建好的动作。</t>
+  </si>
+  <si>
+    <t>注：如果不在queue或者parallel中，每个动作必须有target。如果在queue或者parallel中，没有target的动作将作用于end时声明的target；有target的动作将由该target执行，queue或者parallel仍然有效（如果是queue的话，会衷心地等待该target执行完该动作才继续执行下一个动作）</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1123,6 +1543,11 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1156,7 +1581,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1678,11 +2103,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="285">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1918,6 +2409,207 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="45" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1975,6 +2667,78 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1996,79 +2760,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2114,6 +2809,48 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2185,47 +2922,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2239,38 +2958,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2278,78 +3000,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 2" xfId="1"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -2707,25 +3388,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F144"/>
+  <dimension ref="A1:F241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F175" sqref="F175:F178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="18.625" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="55.375" customWidth="1"/>
     <col min="6" max="6" width="50.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="189" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="99"/>
+      <c r="B1" s="190"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2740,10 +3421,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="191" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="101"/>
+      <c r="B2" s="192"/>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
@@ -2753,13 +3434,13 @@
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="103" t="s">
+      <c r="F2" s="194" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="101"/>
-      <c r="B3" s="101"/>
+      <c r="A3" s="192"/>
+      <c r="B3" s="192"/>
       <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
@@ -2769,11 +3450,11 @@
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="104"/>
+      <c r="F3" s="195"/>
     </row>
     <row r="4" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="102"/>
-      <c r="B4" s="102"/>
+      <c r="A4" s="193"/>
+      <c r="B4" s="193"/>
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
@@ -2783,13 +3464,13 @@
       <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="104"/>
+      <c r="F4" s="195"/>
     </row>
     <row r="5" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="168" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="106"/>
+      <c r="B5" s="169"/>
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
@@ -2799,13 +3480,13 @@
       <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="107" t="s">
+      <c r="F5" s="196" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="91"/>
-      <c r="B6" s="92"/>
+      <c r="A6" s="158"/>
+      <c r="B6" s="159"/>
       <c r="C6" s="8" t="s">
         <v>19</v>
       </c>
@@ -2815,11 +3496,11 @@
       <c r="E6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="107"/>
+      <c r="F6" s="196"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="91"/>
-      <c r="B7" s="92"/>
+      <c r="A7" s="158"/>
+      <c r="B7" s="159"/>
       <c r="C7" s="9" t="s">
         <v>21</v>
       </c>
@@ -2829,11 +3510,11 @@
       <c r="E7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="107"/>
+      <c r="F7" s="196"/>
     </row>
     <row r="8" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="91"/>
-      <c r="B8" s="92"/>
+      <c r="A8" s="158"/>
+      <c r="B8" s="159"/>
       <c r="C8" s="8" t="s">
         <v>23</v>
       </c>
@@ -2843,11 +3524,11 @@
       <c r="E8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="107"/>
+      <c r="F8" s="196"/>
     </row>
     <row r="9" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="91"/>
-      <c r="B9" s="92"/>
+      <c r="A9" s="158"/>
+      <c r="B9" s="159"/>
       <c r="C9" s="9" t="s">
         <v>26</v>
       </c>
@@ -2857,11 +3538,11 @@
       <c r="E9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="107"/>
+      <c r="F9" s="196"/>
     </row>
     <row r="10" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="93"/>
-      <c r="B10" s="94"/>
+      <c r="A10" s="160"/>
+      <c r="B10" s="161"/>
       <c r="C10" s="20" t="s">
         <v>29</v>
       </c>
@@ -2871,13 +3552,13 @@
       <c r="E10" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="107"/>
+      <c r="F10" s="196"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="156" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="90"/>
+      <c r="B11" s="157"/>
       <c r="C11" s="10" t="s">
         <v>6</v>
       </c>
@@ -2887,13 +3568,13 @@
       <c r="E11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="95" t="s">
+      <c r="F11" s="162" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="91"/>
-      <c r="B12" s="92"/>
+      <c r="A12" s="158"/>
+      <c r="B12" s="159"/>
       <c r="C12" s="9" t="s">
         <v>34</v>
       </c>
@@ -2903,11 +3584,11 @@
       <c r="E12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="96"/>
+      <c r="F12" s="163"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="91"/>
-      <c r="B13" s="92"/>
+      <c r="A13" s="158"/>
+      <c r="B13" s="159"/>
       <c r="C13" s="9" t="s">
         <v>36</v>
       </c>
@@ -2917,11 +3598,11 @@
       <c r="E13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="96"/>
+      <c r="F13" s="163"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="91"/>
-      <c r="B14" s="92"/>
+      <c r="A14" s="158"/>
+      <c r="B14" s="159"/>
       <c r="C14" s="9" t="s">
         <v>38</v>
       </c>
@@ -2931,11 +3612,11 @@
       <c r="E14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="96"/>
+      <c r="F14" s="163"/>
     </row>
     <row r="15" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="93"/>
-      <c r="B15" s="94"/>
+      <c r="A15" s="160"/>
+      <c r="B15" s="161"/>
       <c r="C15" s="11" t="s">
         <v>41</v>
       </c>
@@ -2945,13 +3626,13 @@
       <c r="E15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="97"/>
+      <c r="F15" s="164"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="108" t="s">
+      <c r="A16" s="165" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="109"/>
+      <c r="B16" s="166"/>
       <c r="C16" s="10" t="s">
         <v>6</v>
       </c>
@@ -2961,13 +3642,13 @@
       <c r="E16" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="110" t="s">
+      <c r="F16" s="167" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="108"/>
-      <c r="B17" s="109"/>
+      <c r="A17" s="165"/>
+      <c r="B17" s="166"/>
       <c r="C17" s="13" t="s">
         <v>46</v>
       </c>
@@ -2977,13 +3658,13 @@
       <c r="E17" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="110"/>
+      <c r="F17" s="167"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="105" t="s">
+      <c r="A18" s="168" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="106"/>
+      <c r="B18" s="169"/>
       <c r="C18" s="7" t="s">
         <v>6</v>
       </c>
@@ -2993,13 +3674,13 @@
       <c r="E18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="111" t="s">
+      <c r="F18" s="170" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="91"/>
-      <c r="B19" s="92"/>
+      <c r="A19" s="158"/>
+      <c r="B19" s="159"/>
       <c r="C19" s="8" t="s">
         <v>46</v>
       </c>
@@ -3009,11 +3690,11 @@
       <c r="E19" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="95"/>
+      <c r="F19" s="162"/>
     </row>
     <row r="20" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="93"/>
-      <c r="B20" s="94"/>
+      <c r="A20" s="160"/>
+      <c r="B20" s="161"/>
       <c r="C20" s="15" t="s">
         <v>50</v>
       </c>
@@ -3023,13 +3704,13 @@
       <c r="E20" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="97"/>
+      <c r="F20" s="164"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="171" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="113"/>
+      <c r="B21" s="172"/>
       <c r="C21" s="21" t="s">
         <v>10</v>
       </c>
@@ -3039,13 +3720,13 @@
       <c r="E21" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="114" t="s">
+      <c r="F21" s="173" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="112"/>
-      <c r="B22" s="113"/>
+      <c r="A22" s="171"/>
+      <c r="B22" s="172"/>
       <c r="C22" s="22" t="s">
         <v>55</v>
       </c>
@@ -3055,13 +3736,13 @@
       <c r="E22" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="115"/>
+      <c r="F22" s="174"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23" s="125" t="s">
+      <c r="A23" s="184" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="126"/>
+      <c r="B23" s="185"/>
       <c r="C23" s="23" t="s">
         <v>6</v>
       </c>
@@ -3071,13 +3752,13 @@
       <c r="E23" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="127" t="s">
+      <c r="F23" s="186" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="112"/>
-      <c r="B24" s="113"/>
+      <c r="A24" s="171"/>
+      <c r="B24" s="172"/>
       <c r="C24" s="22" t="s">
         <v>55</v>
       </c>
@@ -3087,13 +3768,13 @@
       <c r="E24" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="115"/>
+      <c r="F24" s="174"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="105" t="s">
+      <c r="A25" s="168" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="106"/>
+      <c r="B25" s="169"/>
       <c r="C25" s="16" t="s">
         <v>6</v>
       </c>
@@ -3103,13 +3784,13 @@
       <c r="E25" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F25" s="130" t="s">
+      <c r="F25" s="198" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A26" s="91"/>
-      <c r="B26" s="92"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="158"/>
+      <c r="B26" s="159"/>
       <c r="C26" s="24" t="s">
         <v>64</v>
       </c>
@@ -3119,11 +3800,11 @@
       <c r="E26" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="96"/>
+      <c r="F26" s="163"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A27" s="91"/>
-      <c r="B27" s="92"/>
+      <c r="A27" s="158"/>
+      <c r="B27" s="159"/>
       <c r="C27" s="17" t="s">
         <v>67</v>
       </c>
@@ -3133,11 +3814,11 @@
       <c r="E27" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="96"/>
+      <c r="F27" s="163"/>
     </row>
     <row r="28" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="128"/>
-      <c r="B28" s="129"/>
+      <c r="A28" s="187"/>
+      <c r="B28" s="188"/>
       <c r="C28" s="18" t="s">
         <v>69</v>
       </c>
@@ -3147,13 +3828,13 @@
       <c r="E28" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="F28" s="131"/>
+      <c r="F28" s="199"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A29" s="132" t="s">
+      <c r="A29" s="200" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="133"/>
+      <c r="B29" s="201"/>
       <c r="C29" s="25" t="s">
         <v>6</v>
       </c>
@@ -3163,13 +3844,13 @@
       <c r="E29" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="127" t="s">
+      <c r="F29" s="186" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A30" s="134"/>
-      <c r="B30" s="135"/>
+      <c r="A30" s="202"/>
+      <c r="B30" s="203"/>
       <c r="C30" s="24" t="s">
         <v>64</v>
       </c>
@@ -3179,11 +3860,11 @@
       <c r="E30" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F30" s="115"/>
+      <c r="F30" s="174"/>
     </row>
     <row r="31" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="136"/>
-      <c r="B31" s="137"/>
+      <c r="A31" s="204"/>
+      <c r="B31" s="205"/>
       <c r="C31" s="26" t="s">
         <v>67</v>
       </c>
@@ -3193,13 +3874,13 @@
       <c r="E31" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F31" s="138"/>
+      <c r="F31" s="206"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A32" s="125" t="s">
+      <c r="A32" s="184" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="126"/>
+      <c r="B32" s="185"/>
       <c r="C32" s="25" t="s">
         <v>6</v>
       </c>
@@ -3209,13 +3890,13 @@
       <c r="E32" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="F32" s="141" t="s">
+      <c r="F32" s="209" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33" s="112"/>
-      <c r="B33" s="113"/>
+      <c r="A33" s="171"/>
+      <c r="B33" s="172"/>
       <c r="C33" s="24" t="s">
         <v>79</v>
       </c>
@@ -3225,11 +3906,11 @@
       <c r="E33" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="F33" s="142"/>
+      <c r="F33" s="210"/>
     </row>
     <row r="34" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="112"/>
-      <c r="B34" s="113"/>
+      <c r="A34" s="171"/>
+      <c r="B34" s="172"/>
       <c r="C34" s="28" t="s">
         <v>81</v>
       </c>
@@ -3239,11 +3920,11 @@
       <c r="E34" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="143"/>
+      <c r="F34" s="211"/>
     </row>
     <row r="35" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="139"/>
-      <c r="B35" s="140"/>
+      <c r="A35" s="207"/>
+      <c r="B35" s="208"/>
       <c r="C35" s="29" t="s">
         <v>83</v>
       </c>
@@ -3253,14 +3934,14 @@
       <c r="E35" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="F35" s="144"/>
+      <c r="F35" s="212"/>
     </row>
     <row r="37" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="145" t="s">
+      <c r="A38" s="227" t="s">
         <v>85</v>
       </c>
-      <c r="B38" s="99"/>
+      <c r="B38" s="190"/>
       <c r="C38" s="1" t="s">
         <v>1</v>
       </c>
@@ -3275,10 +3956,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A39" s="116" t="s">
+      <c r="A39" s="175" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="117"/>
+      <c r="B39" s="176"/>
       <c r="C39" s="30" t="s">
         <v>10</v>
       </c>
@@ -3288,13 +3969,13 @@
       <c r="E39" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="F39" s="122" t="s">
+      <c r="F39" s="181" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A40" s="118"/>
-      <c r="B40" s="119"/>
+      <c r="A40" s="177"/>
+      <c r="B40" s="178"/>
       <c r="C40" s="31" t="s">
         <v>89</v>
       </c>
@@ -3304,11 +3985,11 @@
       <c r="E40" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="F40" s="123"/>
+      <c r="F40" s="182"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A41" s="118"/>
-      <c r="B41" s="119"/>
+      <c r="A41" s="177"/>
+      <c r="B41" s="178"/>
       <c r="C41" s="31" t="s">
         <v>91</v>
       </c>
@@ -3318,11 +3999,11 @@
       <c r="E41" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="F41" s="123"/>
+      <c r="F41" s="182"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A42" s="118"/>
-      <c r="B42" s="119"/>
+      <c r="A42" s="177"/>
+      <c r="B42" s="178"/>
       <c r="C42" s="31" t="s">
         <v>94</v>
       </c>
@@ -3332,11 +4013,11 @@
       <c r="E42" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="F42" s="123"/>
+      <c r="F42" s="182"/>
     </row>
     <row r="43" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="120"/>
-      <c r="B43" s="121"/>
+      <c r="A43" s="179"/>
+      <c r="B43" s="180"/>
       <c r="C43" s="20" t="s">
         <v>97</v>
       </c>
@@ -3346,13 +4027,13 @@
       <c r="E43" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="F43" s="124"/>
+      <c r="F43" s="183"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A44" s="116" t="s">
+      <c r="A44" s="175" t="s">
         <v>99</v>
       </c>
-      <c r="B44" s="117"/>
+      <c r="B44" s="176"/>
       <c r="C44" s="30" t="s">
         <v>10</v>
       </c>
@@ -3362,13 +4043,13 @@
       <c r="E44" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="F44" s="122" t="s">
+      <c r="F44" s="181" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A45" s="118"/>
-      <c r="B45" s="119"/>
+      <c r="A45" s="177"/>
+      <c r="B45" s="178"/>
       <c r="C45" s="32" t="s">
         <v>102</v>
       </c>
@@ -3378,11 +4059,11 @@
       <c r="E45" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="F45" s="123"/>
+      <c r="F45" s="182"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A46" s="118"/>
-      <c r="B46" s="119"/>
+      <c r="A46" s="177"/>
+      <c r="B46" s="178"/>
       <c r="C46" s="31" t="s">
         <v>104</v>
       </c>
@@ -3392,11 +4073,11 @@
       <c r="E46" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="F46" s="123"/>
+      <c r="F46" s="182"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A47" s="118"/>
-      <c r="B47" s="119"/>
+      <c r="A47" s="177"/>
+      <c r="B47" s="178"/>
       <c r="C47" s="31" t="s">
         <v>91</v>
       </c>
@@ -3406,11 +4087,11 @@
       <c r="E47" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="F47" s="123"/>
+      <c r="F47" s="182"/>
     </row>
     <row r="48" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="120"/>
-      <c r="B48" s="121"/>
+      <c r="A48" s="179"/>
+      <c r="B48" s="180"/>
       <c r="C48" s="33" t="s">
         <v>94</v>
       </c>
@@ -3420,13 +4101,13 @@
       <c r="E48" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="F48" s="124"/>
+      <c r="F48" s="183"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="116" t="s">
+      <c r="A49" s="175" t="s">
         <v>106</v>
       </c>
-      <c r="B49" s="117"/>
+      <c r="B49" s="176"/>
       <c r="C49" s="30" t="s">
         <v>10</v>
       </c>
@@ -3436,13 +4117,13 @@
       <c r="E49" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="F49" s="122" t="s">
+      <c r="F49" s="181" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="120"/>
-      <c r="B50" s="121"/>
+      <c r="A50" s="179"/>
+      <c r="B50" s="180"/>
       <c r="C50" s="33" t="s">
         <v>91</v>
       </c>
@@ -3452,13 +4133,13 @@
       <c r="E50" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="F50" s="124"/>
+      <c r="F50" s="183"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A51" s="116" t="s">
+      <c r="A51" s="175" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="117"/>
+      <c r="B51" s="176"/>
       <c r="C51" s="30" t="s">
         <v>109</v>
       </c>
@@ -3468,13 +4149,13 @@
       <c r="E51" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="F51" s="122" t="s">
+      <c r="F51" s="181" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="120"/>
-      <c r="B52" s="121"/>
+      <c r="A52" s="179"/>
+      <c r="B52" s="180"/>
       <c r="C52" s="11" t="s">
         <v>112</v>
       </c>
@@ -3484,13 +4165,13 @@
       <c r="E52" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F52" s="124"/>
+      <c r="F52" s="183"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A53" s="116" t="s">
+      <c r="A53" s="175" t="s">
         <v>114</v>
       </c>
-      <c r="B53" s="117"/>
+      <c r="B53" s="176"/>
       <c r="C53" s="30" t="s">
         <v>115</v>
       </c>
@@ -3500,13 +4181,13 @@
       <c r="E53" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="F53" s="122" t="s">
+      <c r="F53" s="181" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A54" s="118"/>
-      <c r="B54" s="119"/>
+      <c r="A54" s="177"/>
+      <c r="B54" s="178"/>
       <c r="C54" s="22" t="s">
         <v>67</v>
       </c>
@@ -3516,11 +4197,11 @@
       <c r="E54" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F54" s="123"/>
+      <c r="F54" s="182"/>
     </row>
     <row r="55" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="120"/>
-      <c r="B55" s="121"/>
+      <c r="A55" s="179"/>
+      <c r="B55" s="180"/>
       <c r="C55" s="33" t="s">
         <v>64</v>
       </c>
@@ -3530,13 +4211,13 @@
       <c r="E55" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="F55" s="124"/>
+      <c r="F55" s="183"/>
     </row>
     <row r="56" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="147" t="s">
+      <c r="A56" s="229" t="s">
         <v>120</v>
       </c>
-      <c r="B56" s="148"/>
+      <c r="B56" s="230"/>
       <c r="C56" s="34" t="s">
         <v>115</v>
       </c>
@@ -3551,10 +4232,10 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="147" t="s">
+      <c r="A57" s="229" t="s">
         <v>123</v>
       </c>
-      <c r="B57" s="148"/>
+      <c r="B57" s="230"/>
       <c r="C57" s="1" t="s">
         <v>115</v>
       </c>
@@ -3569,10 +4250,10 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A58" s="149" t="s">
+      <c r="A58" s="231" t="s">
         <v>126</v>
       </c>
-      <c r="B58" s="150"/>
+      <c r="B58" s="232"/>
       <c r="C58" s="30" t="s">
         <v>115</v>
       </c>
@@ -3582,13 +4263,13 @@
       <c r="E58" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="F58" s="122" t="s">
+      <c r="F58" s="181" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A59" s="151"/>
-      <c r="B59" s="152"/>
+      <c r="A59" s="233"/>
+      <c r="B59" s="234"/>
       <c r="C59" s="31" t="s">
         <v>129</v>
       </c>
@@ -3598,11 +4279,11 @@
       <c r="E59" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="F59" s="123"/>
+      <c r="F59" s="182"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A60" s="151"/>
-      <c r="B60" s="152"/>
+      <c r="A60" s="233"/>
+      <c r="B60" s="234"/>
       <c r="C60" s="31" t="s">
         <v>131</v>
       </c>
@@ -3612,11 +4293,11 @@
       <c r="E60" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="F60" s="123"/>
+      <c r="F60" s="182"/>
     </row>
     <row r="61" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="153"/>
-      <c r="B61" s="154"/>
+      <c r="A61" s="235"/>
+      <c r="B61" s="236"/>
       <c r="C61" s="11" t="s">
         <v>133</v>
       </c>
@@ -3626,7 +4307,7 @@
       <c r="E61" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="F61" s="124"/>
+      <c r="F61" s="183"/>
     </row>
     <row r="63" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
@@ -3650,10 +4331,10 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A65" s="155" t="s">
+      <c r="A65" s="237" t="s">
         <v>137</v>
       </c>
-      <c r="B65" s="158" t="s">
+      <c r="B65" s="240" t="s">
         <v>138</v>
       </c>
       <c r="C65" s="16" t="s">
@@ -3665,13 +4346,13 @@
       <c r="E65" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="F65" s="161" t="s">
+      <c r="F65" s="243" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="156"/>
-      <c r="B66" s="159"/>
+      <c r="A66" s="238"/>
+      <c r="B66" s="241"/>
       <c r="C66" s="44" t="s">
         <v>10</v>
       </c>
@@ -3681,11 +4362,11 @@
       <c r="E66" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="F66" s="162"/>
+      <c r="F66" s="244"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A67" s="156"/>
-      <c r="B67" s="159"/>
+      <c r="A67" s="238"/>
+      <c r="B67" s="241"/>
       <c r="C67" s="44" t="s">
         <v>143</v>
       </c>
@@ -3695,11 +4376,11 @@
       <c r="E67" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="F67" s="162"/>
+      <c r="F67" s="244"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A68" s="156"/>
-      <c r="B68" s="159"/>
+      <c r="A68" s="238"/>
+      <c r="B68" s="241"/>
       <c r="C68" s="44" t="s">
         <v>145</v>
       </c>
@@ -3709,11 +4390,11 @@
       <c r="E68" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="F68" s="162"/>
-    </row>
-    <row r="69" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A69" s="156"/>
-      <c r="B69" s="159"/>
+      <c r="F68" s="244"/>
+    </row>
+    <row r="69" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A69" s="238"/>
+      <c r="B69" s="241"/>
       <c r="C69" s="45" t="s">
         <v>147</v>
       </c>
@@ -3723,11 +4404,11 @@
       <c r="E69" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="F69" s="162"/>
+      <c r="F69" s="244"/>
     </row>
     <row r="70" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="156"/>
-      <c r="B70" s="160"/>
+      <c r="A70" s="238"/>
+      <c r="B70" s="242"/>
       <c r="C70" s="46" t="s">
         <v>150</v>
       </c>
@@ -3737,11 +4418,11 @@
       <c r="E70" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="F70" s="163"/>
+      <c r="F70" s="245"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A71" s="156"/>
-      <c r="B71" s="158" t="s">
+      <c r="A71" s="238"/>
+      <c r="B71" s="240" t="s">
         <v>153</v>
       </c>
       <c r="C71" s="16" t="s">
@@ -3753,13 +4434,13 @@
       <c r="E71" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="F71" s="161" t="s">
+      <c r="F71" s="243" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="156"/>
-      <c r="B72" s="159"/>
+      <c r="A72" s="238"/>
+      <c r="B72" s="241"/>
       <c r="C72" s="44" t="s">
         <v>10</v>
       </c>
@@ -3769,11 +4450,11 @@
       <c r="E72" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="F72" s="162"/>
+      <c r="F72" s="244"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A73" s="156"/>
-      <c r="B73" s="159"/>
+      <c r="A73" s="238"/>
+      <c r="B73" s="241"/>
       <c r="C73" s="44" t="s">
         <v>143</v>
       </c>
@@ -3783,11 +4464,11 @@
       <c r="E73" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="F73" s="162"/>
+      <c r="F73" s="244"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A74" s="156"/>
-      <c r="B74" s="159"/>
+      <c r="A74" s="238"/>
+      <c r="B74" s="241"/>
       <c r="C74" s="44" t="s">
         <v>156</v>
       </c>
@@ -3797,11 +4478,11 @@
       <c r="E74" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="F74" s="162"/>
-    </row>
-    <row r="75" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A75" s="156"/>
-      <c r="B75" s="159"/>
+      <c r="F74" s="244"/>
+    </row>
+    <row r="75" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A75" s="238"/>
+      <c r="B75" s="241"/>
       <c r="C75" s="45" t="s">
         <v>147</v>
       </c>
@@ -3811,11 +4492,11 @@
       <c r="E75" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="F75" s="162"/>
+      <c r="F75" s="244"/>
     </row>
     <row r="76" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="156"/>
-      <c r="B76" s="160"/>
+      <c r="A76" s="238"/>
+      <c r="B76" s="242"/>
       <c r="C76" s="47" t="s">
         <v>150</v>
       </c>
@@ -3825,11 +4506,11 @@
       <c r="E76" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="F76" s="163"/>
+      <c r="F76" s="245"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A77" s="156"/>
-      <c r="B77" s="158" t="s">
+      <c r="A77" s="238"/>
+      <c r="B77" s="240" t="s">
         <v>158</v>
       </c>
       <c r="C77" s="48" t="s">
@@ -3841,13 +4522,13 @@
       <c r="E77" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="F77" s="161" t="s">
+      <c r="F77" s="243" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="156"/>
-      <c r="B78" s="159"/>
+      <c r="A78" s="238"/>
+      <c r="B78" s="241"/>
       <c r="C78" s="44" t="s">
         <v>10</v>
       </c>
@@ -3857,11 +4538,11 @@
       <c r="E78" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="F78" s="162"/>
-    </row>
-    <row r="79" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A79" s="156"/>
-      <c r="B79" s="159"/>
+      <c r="F78" s="244"/>
+    </row>
+    <row r="79" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A79" s="238"/>
+      <c r="B79" s="241"/>
       <c r="C79" s="45" t="s">
         <v>147</v>
       </c>
@@ -3871,11 +4552,11 @@
       <c r="E79" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="F79" s="162"/>
+      <c r="F79" s="244"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A80" s="156"/>
-      <c r="B80" s="159"/>
+      <c r="A80" s="238"/>
+      <c r="B80" s="241"/>
       <c r="C80" s="44" t="s">
         <v>89</v>
       </c>
@@ -3885,11 +4566,11 @@
       <c r="E80" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="F80" s="162"/>
+      <c r="F80" s="244"/>
     </row>
     <row r="81" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="156"/>
-      <c r="B81" s="160"/>
+      <c r="A81" s="238"/>
+      <c r="B81" s="242"/>
       <c r="C81" s="47" t="s">
         <v>163</v>
       </c>
@@ -3899,10 +4580,10 @@
       <c r="E81" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="F81" s="163"/>
+      <c r="F81" s="245"/>
     </row>
     <row r="82" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="156"/>
+      <c r="A82" s="238"/>
       <c r="B82" s="50" t="s">
         <v>165</v>
       </c>
@@ -3920,8 +4601,8 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A83" s="156"/>
-      <c r="B83" s="158" t="s">
+      <c r="A83" s="238"/>
+      <c r="B83" s="240" t="s">
         <v>168</v>
       </c>
       <c r="C83" s="49" t="s">
@@ -3933,13 +4614,13 @@
       <c r="E83" s="49" t="s">
         <v>169</v>
       </c>
-      <c r="F83" s="161" t="s">
+      <c r="F83" s="243" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="156"/>
-      <c r="B84" s="160"/>
+      <c r="A84" s="238"/>
+      <c r="B84" s="242"/>
       <c r="C84" s="47" t="s">
         <v>143</v>
       </c>
@@ -3949,10 +4630,10 @@
       <c r="E84" s="47" t="s">
         <v>171</v>
       </c>
-      <c r="F84" s="163"/>
+      <c r="F84" s="245"/>
     </row>
     <row r="85" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="157"/>
+      <c r="A85" s="239"/>
       <c r="B85" s="54" t="s">
         <v>108</v>
       </c>
@@ -4014,10 +4695,10 @@
       </c>
     </row>
     <row r="93" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="79" t="s">
+      <c r="A93" s="146" t="s">
         <v>174</v>
       </c>
-      <c r="B93" s="80"/>
+      <c r="B93" s="147"/>
       <c r="C93" s="16" t="s">
         <v>6</v>
       </c>
@@ -4027,13 +4708,13 @@
       <c r="E93" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="F93" s="85" t="s">
+      <c r="F93" s="152" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="81"/>
-      <c r="B94" s="82"/>
+      <c r="A94" s="148"/>
+      <c r="B94" s="149"/>
       <c r="C94" s="17" t="s">
         <v>177</v>
       </c>
@@ -4043,11 +4724,11 @@
       <c r="E94" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="F94" s="85"/>
-    </row>
-    <row r="95" spans="1:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="81"/>
-      <c r="B95" s="82"/>
+      <c r="F94" s="152"/>
+    </row>
+    <row r="95" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="148"/>
+      <c r="B95" s="149"/>
       <c r="C95" s="17" t="s">
         <v>179</v>
       </c>
@@ -4057,11 +4738,11 @@
       <c r="E95" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="F95" s="85"/>
+      <c r="F95" s="152"/>
     </row>
     <row r="96" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="81"/>
-      <c r="B96" s="82"/>
+      <c r="A96" s="148"/>
+      <c r="B96" s="149"/>
       <c r="C96" s="17" t="s">
         <v>182</v>
       </c>
@@ -4071,11 +4752,11 @@
       <c r="E96" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="F96" s="85"/>
+      <c r="F96" s="152"/>
     </row>
     <row r="97" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="81"/>
-      <c r="B97" s="82"/>
+      <c r="A97" s="148"/>
+      <c r="B97" s="149"/>
       <c r="C97" s="64" t="s">
         <v>184</v>
       </c>
@@ -4085,11 +4766,11 @@
       <c r="E97" s="64" t="s">
         <v>220</v>
       </c>
-      <c r="F97" s="85"/>
+      <c r="F97" s="152"/>
     </row>
     <row r="98" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="81"/>
-      <c r="B98" s="82"/>
+      <c r="A98" s="148"/>
+      <c r="B98" s="149"/>
       <c r="C98" s="64" t="s">
         <v>185</v>
       </c>
@@ -4099,11 +4780,11 @@
       <c r="E98" s="65" t="s">
         <v>186</v>
       </c>
-      <c r="F98" s="85"/>
+      <c r="F98" s="152"/>
     </row>
     <row r="99" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="81"/>
-      <c r="B99" s="82"/>
+      <c r="A99" s="148"/>
+      <c r="B99" s="149"/>
       <c r="C99" s="64" t="s">
         <v>187</v>
       </c>
@@ -4113,11 +4794,11 @@
       <c r="E99" s="65" t="s">
         <v>188</v>
       </c>
-      <c r="F99" s="85"/>
+      <c r="F99" s="152"/>
     </row>
     <row r="100" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="81"/>
-      <c r="B100" s="82"/>
+      <c r="A100" s="148"/>
+      <c r="B100" s="149"/>
       <c r="C100" s="24" t="s">
         <v>189</v>
       </c>
@@ -4127,11 +4808,11 @@
       <c r="E100" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="F100" s="85"/>
+      <c r="F100" s="152"/>
     </row>
     <row r="101" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="81"/>
-      <c r="B101" s="82"/>
+      <c r="A101" s="148"/>
+      <c r="B101" s="149"/>
       <c r="C101" s="17" t="s">
         <v>191</v>
       </c>
@@ -4141,11 +4822,11 @@
       <c r="E101" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="F101" s="85"/>
+      <c r="F101" s="152"/>
     </row>
     <row r="102" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="81"/>
-      <c r="B102" s="82"/>
+      <c r="A102" s="148"/>
+      <c r="B102" s="149"/>
       <c r="C102" s="17" t="s">
         <v>193</v>
       </c>
@@ -4155,11 +4836,11 @@
       <c r="E102" s="61" t="s">
         <v>194</v>
       </c>
-      <c r="F102" s="85"/>
+      <c r="F102" s="152"/>
     </row>
     <row r="103" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="81"/>
-      <c r="B103" s="82"/>
+      <c r="A103" s="148"/>
+      <c r="B103" s="149"/>
       <c r="C103" s="17" t="s">
         <v>195</v>
       </c>
@@ -4169,11 +4850,11 @@
       <c r="E103" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F103" s="85"/>
+      <c r="F103" s="152"/>
     </row>
     <row r="104" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="81"/>
-      <c r="B104" s="82"/>
+      <c r="A104" s="148"/>
+      <c r="B104" s="149"/>
       <c r="C104" s="17" t="s">
         <v>197</v>
       </c>
@@ -4183,11 +4864,11 @@
       <c r="E104" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="F104" s="85"/>
+      <c r="F104" s="152"/>
     </row>
     <row r="105" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="81"/>
-      <c r="B105" s="82"/>
+      <c r="A105" s="148"/>
+      <c r="B105" s="149"/>
       <c r="C105" s="24" t="s">
         <v>199</v>
       </c>
@@ -4197,11 +4878,11 @@
       <c r="E105" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="F105" s="85"/>
+      <c r="F105" s="152"/>
     </row>
     <row r="106" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="81"/>
-      <c r="B106" s="82"/>
+      <c r="A106" s="148"/>
+      <c r="B106" s="149"/>
       <c r="C106" s="24" t="s">
         <v>201</v>
       </c>
@@ -4211,11 +4892,11 @@
       <c r="E106" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="F106" s="85"/>
+      <c r="F106" s="152"/>
     </row>
     <row r="107" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="81"/>
-      <c r="B107" s="82"/>
+      <c r="A107" s="148"/>
+      <c r="B107" s="149"/>
       <c r="C107" s="44" t="s">
         <v>203</v>
       </c>
@@ -4225,11 +4906,11 @@
       <c r="E107" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="F107" s="85"/>
+      <c r="F107" s="152"/>
     </row>
     <row r="108" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="81"/>
-      <c r="B108" s="82"/>
+      <c r="A108" s="148"/>
+      <c r="B108" s="149"/>
       <c r="C108" s="44" t="s">
         <v>205</v>
       </c>
@@ -4239,11 +4920,11 @@
       <c r="E108" s="44" t="s">
         <v>206</v>
       </c>
-      <c r="F108" s="85"/>
+      <c r="F108" s="152"/>
     </row>
     <row r="109" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="81"/>
-      <c r="B109" s="82"/>
+      <c r="A109" s="148"/>
+      <c r="B109" s="149"/>
       <c r="C109" s="62" t="s">
         <v>207</v>
       </c>
@@ -4253,11 +4934,11 @@
       <c r="E109" s="62" t="s">
         <v>208</v>
       </c>
-      <c r="F109" s="85"/>
+      <c r="F109" s="152"/>
     </row>
     <row r="110" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="83"/>
-      <c r="B110" s="84"/>
+      <c r="A110" s="150"/>
+      <c r="B110" s="151"/>
       <c r="C110" s="63" t="s">
         <v>209</v>
       </c>
@@ -4267,31 +4948,31 @@
       <c r="E110" s="63" t="s">
         <v>210</v>
       </c>
-      <c r="F110" s="85"/>
+      <c r="F110" s="152"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A111" s="146" t="s">
+      <c r="A111" s="228" t="s">
         <v>219</v>
       </c>
-      <c r="B111" s="146"/>
-      <c r="C111" s="146"/>
-      <c r="D111" s="146"/>
-      <c r="E111" s="146"/>
-      <c r="F111" s="146"/>
+      <c r="B111" s="228"/>
+      <c r="C111" s="228"/>
+      <c r="D111" s="228"/>
+      <c r="E111" s="228"/>
+      <c r="F111" s="228"/>
     </row>
     <row r="112" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="146"/>
-      <c r="B112" s="146"/>
-      <c r="C112" s="146"/>
-      <c r="D112" s="146"/>
-      <c r="E112" s="146"/>
-      <c r="F112" s="146"/>
+      <c r="A112" s="228"/>
+      <c r="B112" s="228"/>
+      <c r="C112" s="228"/>
+      <c r="D112" s="228"/>
+      <c r="E112" s="228"/>
+      <c r="F112" s="228"/>
     </row>
     <row r="113" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="79" t="s">
+      <c r="A113" s="146" t="s">
         <v>215</v>
       </c>
-      <c r="B113" s="80"/>
+      <c r="B113" s="147"/>
       <c r="C113" s="74" t="s">
         <v>216</v>
       </c>
@@ -4301,13 +4982,13 @@
       <c r="E113" s="74" t="s">
         <v>220</v>
       </c>
-      <c r="F113" s="85" t="s">
+      <c r="F113" s="152" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="81"/>
-      <c r="B114" s="82"/>
+      <c r="A114" s="148"/>
+      <c r="B114" s="149"/>
       <c r="C114" s="44" t="s">
         <v>182</v>
       </c>
@@ -4317,11 +4998,11 @@
       <c r="E114" s="44" t="s">
         <v>218</v>
       </c>
-      <c r="F114" s="85"/>
-    </row>
-    <row r="115" spans="1:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="81"/>
-      <c r="B115" s="82"/>
+      <c r="F114" s="152"/>
+    </row>
+    <row r="115" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="148"/>
+      <c r="B115" s="149"/>
       <c r="C115" s="44" t="s">
         <v>179</v>
       </c>
@@ -4331,11 +5012,11 @@
       <c r="E115" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="F115" s="85"/>
+      <c r="F115" s="152"/>
     </row>
     <row r="116" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="81"/>
-      <c r="B116" s="82"/>
+      <c r="A116" s="148"/>
+      <c r="B116" s="149"/>
       <c r="C116" s="44" t="s">
         <v>195</v>
       </c>
@@ -4345,11 +5026,11 @@
       <c r="E116" s="44" t="s">
         <v>196</v>
       </c>
-      <c r="F116" s="85"/>
+      <c r="F116" s="152"/>
     </row>
     <row r="117" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="81"/>
-      <c r="B117" s="82"/>
+      <c r="A117" s="148"/>
+      <c r="B117" s="149"/>
       <c r="C117" s="44" t="s">
         <v>197</v>
       </c>
@@ -4359,11 +5040,11 @@
       <c r="E117" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="F117" s="85"/>
+      <c r="F117" s="152"/>
     </row>
     <row r="118" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="81"/>
-      <c r="B118" s="82"/>
+      <c r="A118" s="148"/>
+      <c r="B118" s="149"/>
       <c r="C118" s="62" t="s">
         <v>199</v>
       </c>
@@ -4373,11 +5054,11 @@
       <c r="E118" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="F118" s="85"/>
+      <c r="F118" s="152"/>
     </row>
     <row r="119" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="81"/>
-      <c r="B119" s="82"/>
+      <c r="A119" s="148"/>
+      <c r="B119" s="149"/>
       <c r="C119" s="62" t="s">
         <v>201</v>
       </c>
@@ -4387,11 +5068,11 @@
       <c r="E119" s="62" t="s">
         <v>202</v>
       </c>
-      <c r="F119" s="85"/>
+      <c r="F119" s="152"/>
     </row>
     <row r="120" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="81"/>
-      <c r="B120" s="82"/>
+      <c r="A120" s="148"/>
+      <c r="B120" s="149"/>
       <c r="C120" s="44" t="s">
         <v>203</v>
       </c>
@@ -4401,11 +5082,11 @@
       <c r="E120" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="F120" s="85"/>
+      <c r="F120" s="152"/>
     </row>
     <row r="121" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="81"/>
-      <c r="B121" s="82"/>
+      <c r="A121" s="148"/>
+      <c r="B121" s="149"/>
       <c r="C121" s="44" t="s">
         <v>205</v>
       </c>
@@ -4415,11 +5096,11 @@
       <c r="E121" s="44" t="s">
         <v>206</v>
       </c>
-      <c r="F121" s="85"/>
+      <c r="F121" s="152"/>
     </row>
     <row r="122" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="81"/>
-      <c r="B122" s="82"/>
+      <c r="A122" s="148"/>
+      <c r="B122" s="149"/>
       <c r="C122" s="75" t="s">
         <v>207</v>
       </c>
@@ -4429,11 +5110,11 @@
       <c r="E122" s="75" t="s">
         <v>208</v>
       </c>
-      <c r="F122" s="85"/>
+      <c r="F122" s="152"/>
     </row>
     <row r="123" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="83"/>
-      <c r="B123" s="84"/>
+      <c r="A123" s="150"/>
+      <c r="B123" s="151"/>
       <c r="C123" s="76" t="s">
         <v>209</v>
       </c>
@@ -4443,13 +5124,13 @@
       <c r="E123" s="76" t="s">
         <v>210</v>
       </c>
-      <c r="F123" s="86"/>
+      <c r="F123" s="153"/>
     </row>
     <row r="124" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="87" t="s">
+      <c r="A124" s="154" t="s">
         <v>224</v>
       </c>
-      <c r="B124" s="88"/>
+      <c r="B124" s="155"/>
       <c r="C124" s="77" t="s">
         <v>221</v>
       </c>
@@ -4464,10 +5145,10 @@
       </c>
     </row>
     <row r="125" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="164" t="s">
+      <c r="A125" s="246" t="s">
         <v>225</v>
       </c>
-      <c r="B125" s="165"/>
+      <c r="B125" s="247"/>
       <c r="C125" s="72" t="s">
         <v>6</v>
       </c>
@@ -4477,13 +5158,13 @@
       <c r="E125" s="52" t="s">
         <v>226</v>
       </c>
-      <c r="F125" s="161" t="s">
+      <c r="F125" s="243" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="166"/>
-      <c r="B126" s="167"/>
+      <c r="A126" s="248"/>
+      <c r="B126" s="249"/>
       <c r="C126" s="72" t="s">
         <v>227</v>
       </c>
@@ -4493,11 +5174,11 @@
       <c r="E126" s="52" t="s">
         <v>228</v>
       </c>
-      <c r="F126" s="162"/>
+      <c r="F126" s="244"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A127" s="166"/>
-      <c r="B127" s="167"/>
+      <c r="A127" s="248"/>
+      <c r="B127" s="249"/>
       <c r="C127" s="72" t="s">
         <v>23</v>
       </c>
@@ -4507,65 +5188,65 @@
       <c r="E127" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="F127" s="162"/>
+      <c r="F127" s="244"/>
     </row>
     <row r="128" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="174" t="s">
+      <c r="A128" s="250" t="s">
         <v>230</v>
       </c>
-      <c r="B128" s="175"/>
-      <c r="C128" s="176" t="s">
+      <c r="B128" s="251"/>
+      <c r="C128" s="81" t="s">
         <v>231</v>
       </c>
       <c r="D128" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="E128" s="176" t="s">
+      <c r="E128" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="F128" s="180" t="s">
+      <c r="F128" s="83" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="177" t="s">
+      <c r="A129" s="252" t="s">
         <v>232</v>
       </c>
-      <c r="B129" s="178"/>
-      <c r="C129" s="179" t="s">
+      <c r="B129" s="253"/>
+      <c r="C129" s="82" t="s">
         <v>231</v>
       </c>
       <c r="D129" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="E129" s="179" t="s">
+      <c r="E129" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="F129" s="181" t="s">
+      <c r="F129" s="84" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A130" s="168" t="s">
+      <c r="A130" s="254" t="s">
         <v>233</v>
       </c>
-      <c r="B130" s="169"/>
-      <c r="C130" s="170" t="s">
+      <c r="B130" s="255"/>
+      <c r="C130" s="79" t="s">
         <v>234</v>
       </c>
-      <c r="D130" s="171" t="s">
+      <c r="D130" s="80" t="s">
         <v>235</v>
       </c>
-      <c r="E130" s="170" t="s">
+      <c r="E130" s="79" t="s">
         <v>236</v>
       </c>
-      <c r="F130" s="182" t="s">
+      <c r="F130" s="258" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A131" s="172"/>
-      <c r="B131" s="173"/>
+      <c r="A131" s="256"/>
+      <c r="B131" s="257"/>
       <c r="C131" s="26" t="s">
         <v>237</v>
       </c>
@@ -4575,141 +5256,141 @@
       <c r="E131" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="F131" s="183"/>
+      <c r="F131" s="259"/>
     </row>
     <row r="132" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="184" t="s">
+      <c r="A132" s="260" t="s">
         <v>243</v>
       </c>
-      <c r="B132" s="185"/>
-      <c r="C132" s="186" t="s">
+      <c r="B132" s="261"/>
+      <c r="C132" s="85" t="s">
         <v>244</v>
       </c>
-      <c r="D132" s="186"/>
-      <c r="E132" s="186"/>
-      <c r="F132" s="187" t="s">
+      <c r="D132" s="85"/>
+      <c r="E132" s="85"/>
+      <c r="F132" s="86" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="98" t="s">
+      <c r="A133" s="189" t="s">
         <v>246</v>
       </c>
-      <c r="B133" s="188"/>
-      <c r="C133" s="189" t="s">
+      <c r="B133" s="262"/>
+      <c r="C133" s="87" t="s">
         <v>244</v>
       </c>
-      <c r="D133" s="189"/>
-      <c r="E133" s="189"/>
-      <c r="F133" s="190" t="s">
+      <c r="D133" s="87"/>
+      <c r="E133" s="87"/>
+      <c r="F133" s="88" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="98" t="s">
+      <c r="A134" s="189" t="s">
         <v>248</v>
       </c>
-      <c r="B134" s="188"/>
-      <c r="C134" s="189" t="s">
+      <c r="B134" s="262"/>
+      <c r="C134" s="87" t="s">
         <v>244</v>
       </c>
-      <c r="D134" s="189"/>
-      <c r="E134" s="189"/>
-      <c r="F134" s="190" t="s">
+      <c r="D134" s="87"/>
+      <c r="E134" s="87"/>
+      <c r="F134" s="88" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="98" t="s">
+      <c r="A135" s="189" t="s">
         <v>250</v>
       </c>
-      <c r="B135" s="188"/>
-      <c r="C135" s="189" t="s">
+      <c r="B135" s="262"/>
+      <c r="C135" s="87" t="s">
         <v>244</v>
       </c>
-      <c r="D135" s="189"/>
-      <c r="E135" s="189"/>
-      <c r="F135" s="190" t="s">
+      <c r="D135" s="87"/>
+      <c r="E135" s="87"/>
+      <c r="F135" s="88" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="191" t="s">
+      <c r="A136" s="263" t="s">
         <v>252</v>
       </c>
-      <c r="B136" s="192"/>
-      <c r="C136" s="193" t="s">
+      <c r="B136" s="264"/>
+      <c r="C136" s="89" t="s">
         <v>244</v>
       </c>
-      <c r="D136" s="193"/>
-      <c r="E136" s="193"/>
-      <c r="F136" s="194" t="s">
+      <c r="D136" s="89"/>
+      <c r="E136" s="89"/>
+      <c r="F136" s="90" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="206" t="s">
+      <c r="A137" s="270" t="s">
         <v>254</v>
       </c>
-      <c r="B137" s="207"/>
-      <c r="C137" s="208" t="s">
+      <c r="B137" s="271"/>
+      <c r="C137" s="95" t="s">
         <v>244</v>
       </c>
-      <c r="D137" s="208"/>
-      <c r="E137" s="208"/>
-      <c r="F137" s="209" t="s">
+      <c r="D137" s="95"/>
+      <c r="E137" s="95"/>
+      <c r="F137" s="96" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="210" t="s">
+      <c r="A138" s="272" t="s">
         <v>256</v>
       </c>
-      <c r="B138" s="211"/>
-      <c r="C138" s="208" t="s">
+      <c r="B138" s="273"/>
+      <c r="C138" s="95" t="s">
         <v>244</v>
       </c>
-      <c r="D138" s="208"/>
-      <c r="E138" s="208"/>
-      <c r="F138" s="209" t="s">
+      <c r="D138" s="95"/>
+      <c r="E138" s="95"/>
+      <c r="F138" s="96" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="139" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="197" t="s">
+      <c r="A139" s="274" t="s">
         <v>258</v>
       </c>
-      <c r="B139" s="198"/>
-      <c r="C139" s="195" t="s">
+      <c r="B139" s="275"/>
+      <c r="C139" s="91" t="s">
         <v>244</v>
       </c>
-      <c r="D139" s="195"/>
-      <c r="E139" s="195"/>
-      <c r="F139" s="196" t="s">
+      <c r="D139" s="91"/>
+      <c r="E139" s="91"/>
+      <c r="F139" s="92" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A140" s="212" t="s">
+      <c r="A140" s="276" t="s">
         <v>260</v>
       </c>
-      <c r="B140" s="213"/>
-      <c r="C140" s="214" t="s">
+      <c r="B140" s="277"/>
+      <c r="C140" s="97" t="s">
         <v>177</v>
       </c>
-      <c r="D140" s="214" t="s">
+      <c r="D140" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="E140" s="214" t="s">
+      <c r="E140" s="97" t="s">
         <v>261</v>
       </c>
-      <c r="F140" s="215" t="s">
+      <c r="F140" s="282" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A141" s="216"/>
-      <c r="B141" s="217"/>
+      <c r="A141" s="278"/>
+      <c r="B141" s="279"/>
       <c r="C141" s="24" t="s">
         <v>263</v>
       </c>
@@ -4719,11 +5400,11 @@
       <c r="E141" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="F141" s="218"/>
+      <c r="F141" s="283"/>
     </row>
     <row r="142" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="219"/>
-      <c r="B142" s="220"/>
+      <c r="A142" s="280"/>
+      <c r="B142" s="281"/>
       <c r="C142" s="26" t="s">
         <v>265</v>
       </c>
@@ -4733,42 +5414,1460 @@
       <c r="E142" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="F142" s="221"/>
+      <c r="F142" s="284"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A143" s="199" t="s">
+      <c r="A143" s="265" t="s">
         <v>267</v>
       </c>
-      <c r="B143" s="200"/>
-      <c r="C143" s="201" t="s">
+      <c r="B143" s="266"/>
+      <c r="C143" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="D143" s="201" t="s">
-        <v>7</v>
-      </c>
-      <c r="E143" s="201" t="s">
+      <c r="D143" s="93" t="s">
+        <v>7</v>
+      </c>
+      <c r="E143" s="93" t="s">
         <v>268</v>
       </c>
-      <c r="F143" s="85" t="s">
+      <c r="F143" s="152" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="202"/>
-      <c r="B144" s="203"/>
-      <c r="C144" s="204" t="s">
+      <c r="A144" s="267"/>
+      <c r="B144" s="268"/>
+      <c r="C144" s="94" t="s">
         <v>270</v>
       </c>
-      <c r="D144" s="204" t="s">
+      <c r="D144" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="E144" s="204" t="s">
+      <c r="E144" s="94" t="s">
         <v>271</v>
       </c>
-      <c r="F144" s="205"/>
+      <c r="F144" s="269"/>
+    </row>
+    <row r="145" spans="1:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="197" t="s">
+        <v>272</v>
+      </c>
+      <c r="B145" s="197"/>
+      <c r="C145" s="98" t="s">
+        <v>244</v>
+      </c>
+      <c r="D145" s="98"/>
+      <c r="E145" s="98" t="s">
+        <v>273</v>
+      </c>
+      <c r="F145" s="99" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="197" t="s">
+        <v>275</v>
+      </c>
+      <c r="B146" s="197"/>
+      <c r="C146" s="98" t="s">
+        <v>244</v>
+      </c>
+      <c r="D146" s="98"/>
+      <c r="E146" s="98" t="s">
+        <v>276</v>
+      </c>
+      <c r="F146" s="99"/>
+    </row>
+    <row r="149" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="113"/>
+      <c r="B149" s="114"/>
+      <c r="C149" s="101"/>
+      <c r="D149" s="101"/>
+      <c r="E149" s="101"/>
+      <c r="F149" s="104"/>
+    </row>
+    <row r="150" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="108" t="s">
+        <v>277</v>
+      </c>
+      <c r="B150" s="115" t="s">
+        <v>136</v>
+      </c>
+      <c r="C150" s="116" t="s">
+        <v>1</v>
+      </c>
+      <c r="D150" s="116" t="s">
+        <v>2</v>
+      </c>
+      <c r="E150" s="116" t="s">
+        <v>3</v>
+      </c>
+      <c r="F150" s="117" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="224" t="s">
+        <v>278</v>
+      </c>
+      <c r="B151" s="118" t="s">
+        <v>279</v>
+      </c>
+      <c r="C151" s="119" t="s">
+        <v>244</v>
+      </c>
+      <c r="D151" s="119"/>
+      <c r="E151" s="119"/>
+      <c r="F151" s="120" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="225"/>
+      <c r="B152" s="121" t="s">
+        <v>281</v>
+      </c>
+      <c r="C152" s="109" t="s">
+        <v>244</v>
+      </c>
+      <c r="D152" s="109"/>
+      <c r="E152" s="109"/>
+      <c r="F152" s="110" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A153" s="225"/>
+      <c r="B153" s="217" t="s">
+        <v>283</v>
+      </c>
+      <c r="C153" s="122" t="s">
+        <v>284</v>
+      </c>
+      <c r="D153" s="122" t="s">
+        <v>24</v>
+      </c>
+      <c r="E153" s="122" t="s">
+        <v>285</v>
+      </c>
+      <c r="F153" s="135" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A154" s="225"/>
+      <c r="B154" s="217"/>
+      <c r="C154" s="106" t="s">
+        <v>287</v>
+      </c>
+      <c r="D154" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="E154" s="106" t="s">
+        <v>288</v>
+      </c>
+      <c r="F154" s="135"/>
+    </row>
+    <row r="155" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A155" s="225"/>
+      <c r="B155" s="217"/>
+      <c r="C155" s="106" t="s">
+        <v>289</v>
+      </c>
+      <c r="D155" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E155" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="F155" s="135"/>
+    </row>
+    <row r="156" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="225"/>
+      <c r="B156" s="217"/>
+      <c r="C156" s="107" t="s">
+        <v>291</v>
+      </c>
+      <c r="D156" s="107" t="s">
+        <v>292</v>
+      </c>
+      <c r="E156" s="107" t="s">
+        <v>293</v>
+      </c>
+      <c r="F156" s="135"/>
+    </row>
+    <row r="157" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A157" s="225"/>
+      <c r="B157" s="143" t="s">
+        <v>294</v>
+      </c>
+      <c r="C157" s="105" t="s">
+        <v>284</v>
+      </c>
+      <c r="D157" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="E157" s="105" t="s">
+        <v>295</v>
+      </c>
+      <c r="F157" s="132" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A158" s="225"/>
+      <c r="B158" s="144"/>
+      <c r="C158" s="106" t="s">
+        <v>231</v>
+      </c>
+      <c r="D158" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="E158" s="106" t="s">
+        <v>288</v>
+      </c>
+      <c r="F158" s="136"/>
+    </row>
+    <row r="159" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A159" s="225"/>
+      <c r="B159" s="144"/>
+      <c r="C159" s="106" t="s">
+        <v>289</v>
+      </c>
+      <c r="D159" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E159" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="F159" s="136"/>
+    </row>
+    <row r="160" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="225"/>
+      <c r="B160" s="218"/>
+      <c r="C160" s="107" t="s">
+        <v>291</v>
+      </c>
+      <c r="D160" s="107" t="s">
+        <v>292</v>
+      </c>
+      <c r="E160" s="107" t="s">
+        <v>293</v>
+      </c>
+      <c r="F160" s="133"/>
+    </row>
+    <row r="161" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A161" s="225"/>
+      <c r="B161" s="143" t="s">
+        <v>297</v>
+      </c>
+      <c r="C161" s="105" t="s">
+        <v>298</v>
+      </c>
+      <c r="D161" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="E161" s="105" t="s">
+        <v>299</v>
+      </c>
+      <c r="F161" s="132" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A162" s="225"/>
+      <c r="B162" s="144"/>
+      <c r="C162" s="106" t="s">
+        <v>231</v>
+      </c>
+      <c r="D162" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="E162" s="106" t="s">
+        <v>288</v>
+      </c>
+      <c r="F162" s="136"/>
+    </row>
+    <row r="163" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A163" s="225"/>
+      <c r="B163" s="144"/>
+      <c r="C163" s="106" t="s">
+        <v>289</v>
+      </c>
+      <c r="D163" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E163" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="F163" s="136"/>
+    </row>
+    <row r="164" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="225"/>
+      <c r="B164" s="145"/>
+      <c r="C164" s="103" t="s">
+        <v>291</v>
+      </c>
+      <c r="D164" s="103" t="s">
+        <v>292</v>
+      </c>
+      <c r="E164" s="103" t="s">
+        <v>293</v>
+      </c>
+      <c r="F164" s="137"/>
+    </row>
+    <row r="165" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A165" s="225"/>
+      <c r="B165" s="216" t="s">
+        <v>301</v>
+      </c>
+      <c r="C165" s="111" t="s">
+        <v>231</v>
+      </c>
+      <c r="D165" s="111" t="s">
+        <v>95</v>
+      </c>
+      <c r="E165" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="F165" s="134" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A166" s="225"/>
+      <c r="B166" s="217"/>
+      <c r="C166" s="106" t="s">
+        <v>304</v>
+      </c>
+      <c r="D166" s="106" t="s">
+        <v>305</v>
+      </c>
+      <c r="E166" s="106" t="s">
+        <v>306</v>
+      </c>
+      <c r="F166" s="135"/>
+    </row>
+    <row r="167" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A167" s="225"/>
+      <c r="B167" s="217"/>
+      <c r="C167" s="106" t="s">
+        <v>307</v>
+      </c>
+      <c r="D167" s="106" t="s">
+        <v>305</v>
+      </c>
+      <c r="E167" s="106" t="s">
+        <v>308</v>
+      </c>
+      <c r="F167" s="135"/>
+    </row>
+    <row r="168" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A168" s="225"/>
+      <c r="B168" s="217"/>
+      <c r="C168" s="107" t="s">
+        <v>289</v>
+      </c>
+      <c r="D168" s="107" t="s">
+        <v>7</v>
+      </c>
+      <c r="E168" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="F168" s="135"/>
+    </row>
+    <row r="169" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="225"/>
+      <c r="B169" s="223"/>
+      <c r="C169" s="103" t="s">
+        <v>291</v>
+      </c>
+      <c r="D169" s="103" t="s">
+        <v>292</v>
+      </c>
+      <c r="E169" s="103" t="s">
+        <v>293</v>
+      </c>
+      <c r="F169" s="222"/>
+    </row>
+    <row r="170" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A170" s="225"/>
+      <c r="B170" s="216" t="s">
+        <v>309</v>
+      </c>
+      <c r="C170" s="105" t="s">
+        <v>231</v>
+      </c>
+      <c r="D170" s="105" t="s">
+        <v>95</v>
+      </c>
+      <c r="E170" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="F170" s="134" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A171" s="225"/>
+      <c r="B171" s="217"/>
+      <c r="C171" s="106" t="s">
+        <v>304</v>
+      </c>
+      <c r="D171" s="106" t="s">
+        <v>305</v>
+      </c>
+      <c r="E171" s="106" t="s">
+        <v>306</v>
+      </c>
+      <c r="F171" s="135"/>
+    </row>
+    <row r="172" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A172" s="225"/>
+      <c r="B172" s="217"/>
+      <c r="C172" s="106" t="s">
+        <v>307</v>
+      </c>
+      <c r="D172" s="106" t="s">
+        <v>305</v>
+      </c>
+      <c r="E172" s="106" t="s">
+        <v>308</v>
+      </c>
+      <c r="F172" s="135"/>
+    </row>
+    <row r="173" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A173" s="225"/>
+      <c r="B173" s="217"/>
+      <c r="C173" s="106" t="s">
+        <v>289</v>
+      </c>
+      <c r="D173" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E173" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="F173" s="135"/>
+    </row>
+    <row r="174" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="225"/>
+      <c r="B174" s="217"/>
+      <c r="C174" s="107" t="s">
+        <v>291</v>
+      </c>
+      <c r="D174" s="107" t="s">
+        <v>292</v>
+      </c>
+      <c r="E174" s="107" t="s">
+        <v>293</v>
+      </c>
+      <c r="F174" s="135"/>
+    </row>
+    <row r="175" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A175" s="225"/>
+      <c r="B175" s="143" t="s">
+        <v>311</v>
+      </c>
+      <c r="C175" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="D175" s="105" t="s">
+        <v>7</v>
+      </c>
+      <c r="E175" s="105" t="s">
+        <v>313</v>
+      </c>
+      <c r="F175" s="132" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A176" s="225"/>
+      <c r="B176" s="144"/>
+      <c r="C176" s="106" t="s">
+        <v>231</v>
+      </c>
+      <c r="D176" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="E176" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="F176" s="136"/>
+    </row>
+    <row r="177" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A177" s="225"/>
+      <c r="B177" s="144"/>
+      <c r="C177" s="106" t="s">
+        <v>289</v>
+      </c>
+      <c r="D177" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E177" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="F177" s="136"/>
+    </row>
+    <row r="178" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="225"/>
+      <c r="B178" s="218"/>
+      <c r="C178" s="107" t="s">
+        <v>291</v>
+      </c>
+      <c r="D178" s="107" t="s">
+        <v>292</v>
+      </c>
+      <c r="E178" s="107" t="s">
+        <v>293</v>
+      </c>
+      <c r="F178" s="133"/>
+    </row>
+    <row r="179" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A179" s="225"/>
+      <c r="B179" s="216" t="s">
+        <v>315</v>
+      </c>
+      <c r="C179" s="119" t="s">
+        <v>312</v>
+      </c>
+      <c r="D179" s="119" t="s">
+        <v>7</v>
+      </c>
+      <c r="E179" s="119" t="s">
+        <v>316</v>
+      </c>
+      <c r="F179" s="132" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A180" s="225"/>
+      <c r="B180" s="217"/>
+      <c r="C180" s="106" t="s">
+        <v>231</v>
+      </c>
+      <c r="D180" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="E180" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="F180" s="136"/>
+    </row>
+    <row r="181" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A181" s="225"/>
+      <c r="B181" s="217"/>
+      <c r="C181" s="106" t="s">
+        <v>289</v>
+      </c>
+      <c r="D181" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E181" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="F181" s="136"/>
+    </row>
+    <row r="182" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="225"/>
+      <c r="B182" s="223"/>
+      <c r="C182" s="103" t="s">
+        <v>291</v>
+      </c>
+      <c r="D182" s="103" t="s">
+        <v>292</v>
+      </c>
+      <c r="E182" s="103" t="s">
+        <v>293</v>
+      </c>
+      <c r="F182" s="137"/>
+    </row>
+    <row r="183" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A183" s="225"/>
+      <c r="B183" s="217" t="s">
+        <v>318</v>
+      </c>
+      <c r="C183" s="111" t="s">
+        <v>319</v>
+      </c>
+      <c r="D183" s="111" t="s">
+        <v>7</v>
+      </c>
+      <c r="E183" s="111" t="s">
+        <v>320</v>
+      </c>
+      <c r="F183" s="135" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A184" s="225"/>
+      <c r="B184" s="217"/>
+      <c r="C184" s="106" t="s">
+        <v>322</v>
+      </c>
+      <c r="D184" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E184" s="106" t="s">
+        <v>323</v>
+      </c>
+      <c r="F184" s="135"/>
+    </row>
+    <row r="185" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A185" s="225"/>
+      <c r="B185" s="217"/>
+      <c r="C185" s="107" t="s">
+        <v>324</v>
+      </c>
+      <c r="D185" s="107" t="s">
+        <v>7</v>
+      </c>
+      <c r="E185" s="107" t="s">
+        <v>325</v>
+      </c>
+      <c r="F185" s="135"/>
+    </row>
+    <row r="186" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A186" s="225"/>
+      <c r="B186" s="217"/>
+      <c r="C186" s="106" t="s">
+        <v>231</v>
+      </c>
+      <c r="D186" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="E186" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="F186" s="135"/>
+    </row>
+    <row r="187" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A187" s="225"/>
+      <c r="B187" s="217"/>
+      <c r="C187" s="106" t="s">
+        <v>289</v>
+      </c>
+      <c r="D187" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E187" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="F187" s="135"/>
+    </row>
+    <row r="188" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="225"/>
+      <c r="B188" s="223"/>
+      <c r="C188" s="103" t="s">
+        <v>291</v>
+      </c>
+      <c r="D188" s="103" t="s">
+        <v>292</v>
+      </c>
+      <c r="E188" s="103" t="s">
+        <v>293</v>
+      </c>
+      <c r="F188" s="222"/>
+    </row>
+    <row r="189" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A189" s="225"/>
+      <c r="B189" s="143" t="s">
+        <v>326</v>
+      </c>
+      <c r="C189" s="105" t="s">
+        <v>327</v>
+      </c>
+      <c r="D189" s="105" t="s">
+        <v>7</v>
+      </c>
+      <c r="E189" s="105" t="s">
+        <v>328</v>
+      </c>
+      <c r="F189" s="132" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A190" s="225"/>
+      <c r="B190" s="144"/>
+      <c r="C190" s="106" t="s">
+        <v>231</v>
+      </c>
+      <c r="D190" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="E190" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="F190" s="136"/>
+    </row>
+    <row r="191" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A191" s="225"/>
+      <c r="B191" s="144"/>
+      <c r="C191" s="106" t="s">
+        <v>289</v>
+      </c>
+      <c r="D191" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E191" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="F191" s="136"/>
+    </row>
+    <row r="192" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="225"/>
+      <c r="B192" s="145"/>
+      <c r="C192" s="103" t="s">
+        <v>291</v>
+      </c>
+      <c r="D192" s="103" t="s">
+        <v>292</v>
+      </c>
+      <c r="E192" s="103" t="s">
+        <v>293</v>
+      </c>
+      <c r="F192" s="137"/>
+    </row>
+    <row r="193" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A193" s="225"/>
+      <c r="B193" s="216" t="s">
+        <v>330</v>
+      </c>
+      <c r="C193" s="105" t="s">
+        <v>129</v>
+      </c>
+      <c r="D193" s="105" t="s">
+        <v>95</v>
+      </c>
+      <c r="E193" s="105" t="s">
+        <v>331</v>
+      </c>
+      <c r="F193" s="134" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A194" s="225"/>
+      <c r="B194" s="217"/>
+      <c r="C194" s="106" t="s">
+        <v>36</v>
+      </c>
+      <c r="D194" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E194" s="106" t="s">
+        <v>333</v>
+      </c>
+      <c r="F194" s="135"/>
+    </row>
+    <row r="195" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A195" s="225"/>
+      <c r="B195" s="217"/>
+      <c r="C195" s="106" t="s">
+        <v>334</v>
+      </c>
+      <c r="D195" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E195" s="106" t="s">
+        <v>335</v>
+      </c>
+      <c r="F195" s="135"/>
+    </row>
+    <row r="196" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A196" s="225"/>
+      <c r="B196" s="217"/>
+      <c r="C196" s="106" t="s">
+        <v>289</v>
+      </c>
+      <c r="D196" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E196" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="F196" s="135"/>
+    </row>
+    <row r="197" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="225"/>
+      <c r="B197" s="223"/>
+      <c r="C197" s="103" t="s">
+        <v>336</v>
+      </c>
+      <c r="D197" s="103" t="s">
+        <v>7</v>
+      </c>
+      <c r="E197" s="103" t="s">
+        <v>337</v>
+      </c>
+      <c r="F197" s="222"/>
+    </row>
+    <row r="198" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A198" s="225"/>
+      <c r="B198" s="216" t="s">
+        <v>338</v>
+      </c>
+      <c r="C198" s="105" t="s">
+        <v>129</v>
+      </c>
+      <c r="D198" s="105" t="s">
+        <v>95</v>
+      </c>
+      <c r="E198" s="105" t="s">
+        <v>339</v>
+      </c>
+      <c r="F198" s="134" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A199" s="225"/>
+      <c r="B199" s="217"/>
+      <c r="C199" s="106" t="s">
+        <v>341</v>
+      </c>
+      <c r="D199" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E199" s="106" t="s">
+        <v>342</v>
+      </c>
+      <c r="F199" s="135"/>
+    </row>
+    <row r="200" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A200" s="225"/>
+      <c r="B200" s="217"/>
+      <c r="C200" s="106" t="s">
+        <v>343</v>
+      </c>
+      <c r="D200" s="106" t="s">
+        <v>70</v>
+      </c>
+      <c r="E200" s="106" t="s">
+        <v>344</v>
+      </c>
+      <c r="F200" s="135"/>
+    </row>
+    <row r="201" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A201" s="225"/>
+      <c r="B201" s="217"/>
+      <c r="C201" s="106" t="s">
+        <v>289</v>
+      </c>
+      <c r="D201" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E201" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="F201" s="135"/>
+    </row>
+    <row r="202" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="225"/>
+      <c r="B202" s="223"/>
+      <c r="C202" s="103" t="s">
+        <v>336</v>
+      </c>
+      <c r="D202" s="103" t="s">
+        <v>7</v>
+      </c>
+      <c r="E202" s="103" t="s">
+        <v>337</v>
+      </c>
+      <c r="F202" s="222"/>
+    </row>
+    <row r="203" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A203" s="225"/>
+      <c r="B203" s="216" t="s">
+        <v>345</v>
+      </c>
+      <c r="C203" s="105" t="s">
+        <v>129</v>
+      </c>
+      <c r="D203" s="105" t="s">
+        <v>95</v>
+      </c>
+      <c r="E203" s="105" t="s">
+        <v>339</v>
+      </c>
+      <c r="F203" s="134" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A204" s="225"/>
+      <c r="B204" s="217"/>
+      <c r="C204" s="111" t="s">
+        <v>347</v>
+      </c>
+      <c r="D204" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E204" s="106" t="s">
+        <v>348</v>
+      </c>
+      <c r="F204" s="135"/>
+    </row>
+    <row r="205" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A205" s="225"/>
+      <c r="B205" s="217"/>
+      <c r="C205" s="106" t="s">
+        <v>349</v>
+      </c>
+      <c r="D205" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E205" s="106" t="s">
+        <v>350</v>
+      </c>
+      <c r="F205" s="135"/>
+    </row>
+    <row r="206" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A206" s="225"/>
+      <c r="B206" s="217"/>
+      <c r="C206" s="107" t="s">
+        <v>351</v>
+      </c>
+      <c r="D206" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E206" s="107" t="s">
+        <v>352</v>
+      </c>
+      <c r="F206" s="135"/>
+    </row>
+    <row r="207" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="225"/>
+      <c r="B207" s="217"/>
+      <c r="C207" s="107" t="s">
+        <v>289</v>
+      </c>
+      <c r="D207" s="107" t="s">
+        <v>7</v>
+      </c>
+      <c r="E207" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="F207" s="135"/>
+    </row>
+    <row r="208" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A208" s="225"/>
+      <c r="B208" s="143" t="s">
+        <v>353</v>
+      </c>
+      <c r="C208" s="105" t="s">
+        <v>354</v>
+      </c>
+      <c r="D208" s="102" t="s">
+        <v>70</v>
+      </c>
+      <c r="E208" s="105" t="s">
+        <v>355</v>
+      </c>
+      <c r="F208" s="132" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A209" s="225"/>
+      <c r="B209" s="218"/>
+      <c r="C209" s="107" t="s">
+        <v>289</v>
+      </c>
+      <c r="D209" s="107" t="s">
+        <v>7</v>
+      </c>
+      <c r="E209" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="F209" s="133"/>
+    </row>
+    <row r="210" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A210" s="225"/>
+      <c r="B210" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="C210" s="105" t="s">
+        <v>357</v>
+      </c>
+      <c r="D210" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="E210" s="105" t="s">
+        <v>358</v>
+      </c>
+      <c r="F210" s="132" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="225"/>
+      <c r="B211" s="218"/>
+      <c r="C211" s="107" t="s">
+        <v>289</v>
+      </c>
+      <c r="D211" s="107" t="s">
+        <v>7</v>
+      </c>
+      <c r="E211" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="F211" s="133"/>
+    </row>
+    <row r="212" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A212" s="225"/>
+      <c r="B212" s="143" t="s">
+        <v>360</v>
+      </c>
+      <c r="C212" s="105" t="s">
+        <v>361</v>
+      </c>
+      <c r="D212" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="E212" s="105" t="s">
+        <v>362</v>
+      </c>
+      <c r="F212" s="132" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="225"/>
+      <c r="B213" s="218"/>
+      <c r="C213" s="107" t="s">
+        <v>289</v>
+      </c>
+      <c r="D213" s="107" t="s">
+        <v>7</v>
+      </c>
+      <c r="E213" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="F213" s="133"/>
+    </row>
+    <row r="214" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A214" s="225"/>
+      <c r="B214" s="143" t="s">
+        <v>364</v>
+      </c>
+      <c r="C214" s="105" t="s">
+        <v>361</v>
+      </c>
+      <c r="D214" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="E214" s="105" t="s">
+        <v>362</v>
+      </c>
+      <c r="F214" s="132" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="225"/>
+      <c r="B215" s="218"/>
+      <c r="C215" s="107" t="s">
+        <v>289</v>
+      </c>
+      <c r="D215" s="107" t="s">
+        <v>7</v>
+      </c>
+      <c r="E215" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="F215" s="133"/>
+    </row>
+    <row r="216" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A216" s="225"/>
+      <c r="B216" s="216" t="s">
+        <v>366</v>
+      </c>
+      <c r="C216" s="105" t="s">
+        <v>367</v>
+      </c>
+      <c r="D216" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="E216" s="105" t="s">
+        <v>368</v>
+      </c>
+      <c r="F216" s="134" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A217" s="225"/>
+      <c r="B217" s="217"/>
+      <c r="C217" s="106" t="s">
+        <v>231</v>
+      </c>
+      <c r="D217" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="E217" s="106" t="s">
+        <v>302</v>
+      </c>
+      <c r="F217" s="135"/>
+    </row>
+    <row r="218" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A218" s="225"/>
+      <c r="B218" s="217"/>
+      <c r="C218" s="106" t="s">
+        <v>289</v>
+      </c>
+      <c r="D218" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E218" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="F218" s="135"/>
+    </row>
+    <row r="219" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="225"/>
+      <c r="B219" s="217"/>
+      <c r="C219" s="107" t="s">
+        <v>291</v>
+      </c>
+      <c r="D219" s="107" t="s">
+        <v>292</v>
+      </c>
+      <c r="E219" s="107" t="s">
+        <v>293</v>
+      </c>
+      <c r="F219" s="135"/>
+    </row>
+    <row r="220" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A220" s="225"/>
+      <c r="B220" s="143" t="s">
+        <v>370</v>
+      </c>
+      <c r="C220" s="105" t="s">
+        <v>367</v>
+      </c>
+      <c r="D220" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="E220" s="105" t="s">
+        <v>368</v>
+      </c>
+      <c r="F220" s="132" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A221" s="225"/>
+      <c r="B221" s="144"/>
+      <c r="C221" s="106" t="s">
+        <v>231</v>
+      </c>
+      <c r="D221" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="E221" s="106" t="s">
+        <v>302</v>
+      </c>
+      <c r="F221" s="136"/>
+    </row>
+    <row r="222" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A222" s="225"/>
+      <c r="B222" s="144"/>
+      <c r="C222" s="106" t="s">
+        <v>289</v>
+      </c>
+      <c r="D222" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E222" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="F222" s="136"/>
+    </row>
+    <row r="223" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A223" s="225"/>
+      <c r="B223" s="145"/>
+      <c r="C223" s="103" t="s">
+        <v>291</v>
+      </c>
+      <c r="D223" s="103" t="s">
+        <v>292</v>
+      </c>
+      <c r="E223" s="103" t="s">
+        <v>293</v>
+      </c>
+      <c r="F223" s="137"/>
+    </row>
+    <row r="224" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A224" s="225"/>
+      <c r="B224" s="123" t="s">
+        <v>372</v>
+      </c>
+      <c r="C224" s="122" t="s">
+        <v>129</v>
+      </c>
+      <c r="D224" s="122" t="s">
+        <v>95</v>
+      </c>
+      <c r="E224" s="122" t="s">
+        <v>373</v>
+      </c>
+      <c r="F224" s="124" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A225" s="225"/>
+      <c r="B225" s="143" t="s">
+        <v>375</v>
+      </c>
+      <c r="C225" s="105" t="s">
+        <v>376</v>
+      </c>
+      <c r="D225" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="E225" s="105" t="s">
+        <v>377</v>
+      </c>
+      <c r="F225" s="132" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="225"/>
+      <c r="B226" s="144"/>
+      <c r="C226" s="106" t="s">
+        <v>237</v>
+      </c>
+      <c r="D226" s="106" t="s">
+        <v>11</v>
+      </c>
+      <c r="E226" s="106" t="s">
+        <v>379</v>
+      </c>
+      <c r="F226" s="132"/>
+    </row>
+    <row r="227" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A227" s="225"/>
+      <c r="B227" s="144"/>
+      <c r="C227" s="106" t="s">
+        <v>380</v>
+      </c>
+      <c r="D227" s="106" t="s">
+        <v>11</v>
+      </c>
+      <c r="E227" s="106" t="s">
+        <v>381</v>
+      </c>
+      <c r="F227" s="132"/>
+    </row>
+    <row r="228" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A228" s="225"/>
+      <c r="B228" s="144"/>
+      <c r="C228" s="106" t="s">
+        <v>382</v>
+      </c>
+      <c r="D228" s="106" t="s">
+        <v>383</v>
+      </c>
+      <c r="E228" s="106" t="s">
+        <v>384</v>
+      </c>
+      <c r="F228" s="132"/>
+    </row>
+    <row r="229" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A229" s="225"/>
+      <c r="B229" s="145"/>
+      <c r="C229" s="103" t="s">
+        <v>385</v>
+      </c>
+      <c r="D229" s="103" t="s">
+        <v>70</v>
+      </c>
+      <c r="E229" s="103" t="s">
+        <v>386</v>
+      </c>
+      <c r="F229" s="132"/>
+    </row>
+    <row r="230" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A230" s="225"/>
+      <c r="B230" s="219" t="s">
+        <v>387</v>
+      </c>
+      <c r="C230" s="125" t="s">
+        <v>129</v>
+      </c>
+      <c r="D230" s="105" t="s">
+        <v>95</v>
+      </c>
+      <c r="E230" s="126" t="s">
+        <v>388</v>
+      </c>
+      <c r="F230" s="138" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A231" s="225"/>
+      <c r="B231" s="220"/>
+      <c r="C231" s="112" t="s">
+        <v>390</v>
+      </c>
+      <c r="D231" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E231" s="112" t="s">
+        <v>391</v>
+      </c>
+      <c r="F231" s="139"/>
+    </row>
+    <row r="232" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A232" s="225"/>
+      <c r="B232" s="220"/>
+      <c r="C232" s="112" t="s">
+        <v>392</v>
+      </c>
+      <c r="D232" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E232" s="112" t="s">
+        <v>393</v>
+      </c>
+      <c r="F232" s="139"/>
+    </row>
+    <row r="233" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A233" s="225"/>
+      <c r="B233" s="220"/>
+      <c r="C233" s="112" t="s">
+        <v>394</v>
+      </c>
+      <c r="D233" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E233" s="112" t="s">
+        <v>395</v>
+      </c>
+      <c r="F233" s="139"/>
+    </row>
+    <row r="234" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A234" s="225"/>
+      <c r="B234" s="220"/>
+      <c r="C234" s="112" t="s">
+        <v>351</v>
+      </c>
+      <c r="D234" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E234" s="106" t="s">
+        <v>352</v>
+      </c>
+      <c r="F234" s="139"/>
+    </row>
+    <row r="235" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A235" s="225"/>
+      <c r="B235" s="221"/>
+      <c r="C235" s="103" t="s">
+        <v>289</v>
+      </c>
+      <c r="D235" s="103" t="s">
+        <v>7</v>
+      </c>
+      <c r="E235" s="103" t="s">
+        <v>290</v>
+      </c>
+      <c r="F235" s="140"/>
+    </row>
+    <row r="236" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A236" s="225"/>
+      <c r="B236" s="219" t="s">
+        <v>396</v>
+      </c>
+      <c r="C236" s="126" t="s">
+        <v>289</v>
+      </c>
+      <c r="D236" s="127" t="s">
+        <v>7</v>
+      </c>
+      <c r="E236" s="128" t="s">
+        <v>397</v>
+      </c>
+      <c r="F236" s="140" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A237" s="226"/>
+      <c r="B237" s="221"/>
+      <c r="C237" s="103" t="s">
+        <v>336</v>
+      </c>
+      <c r="D237" s="129" t="s">
+        <v>7</v>
+      </c>
+      <c r="E237" s="130" t="s">
+        <v>399</v>
+      </c>
+      <c r="F237" s="141"/>
+    </row>
+    <row r="238" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A238" s="226"/>
+      <c r="B238" s="219" t="s">
+        <v>165</v>
+      </c>
+      <c r="C238" s="126" t="s">
+        <v>19</v>
+      </c>
+      <c r="D238" s="126" t="s">
+        <v>7</v>
+      </c>
+      <c r="E238" s="126" t="s">
+        <v>397</v>
+      </c>
+      <c r="F238" s="142" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A239" s="226"/>
+      <c r="B239" s="221"/>
+      <c r="C239" s="103" t="s">
+        <v>336</v>
+      </c>
+      <c r="D239" s="131" t="s">
+        <v>7</v>
+      </c>
+      <c r="E239" s="103" t="s">
+        <v>399</v>
+      </c>
+      <c r="F239" s="141"/>
+    </row>
+    <row r="240" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="213" t="s">
+        <v>401</v>
+      </c>
+      <c r="B240" s="214"/>
+      <c r="C240" s="214"/>
+      <c r="D240" s="214"/>
+      <c r="E240" s="214"/>
+      <c r="F240" s="215"/>
+    </row>
+    <row r="241" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A241" s="100"/>
+      <c r="B241" s="100"/>
+      <c r="C241" s="100"/>
+      <c r="D241" s="100"/>
+      <c r="E241" s="100"/>
+      <c r="F241" s="100"/>
     </row>
   </sheetData>
-  <mergeCells count="69">
+  <mergeCells count="117">
+    <mergeCell ref="F212:F213"/>
+    <mergeCell ref="F208:F209"/>
     <mergeCell ref="A143:B144"/>
     <mergeCell ref="F143:F144"/>
     <mergeCell ref="A137:B137"/>
@@ -4776,18 +6875,16 @@
     <mergeCell ref="A139:B139"/>
     <mergeCell ref="A140:B142"/>
     <mergeCell ref="F140:F142"/>
+    <mergeCell ref="F210:F211"/>
+    <mergeCell ref="F189:F192"/>
     <mergeCell ref="A132:B132"/>
     <mergeCell ref="A133:B133"/>
     <mergeCell ref="A134:B134"/>
     <mergeCell ref="A135:B135"/>
     <mergeCell ref="A136:B136"/>
-    <mergeCell ref="A125:B127"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A130:B131"/>
-    <mergeCell ref="F125:F127"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="A111:F112"/>
+    <mergeCell ref="F193:F197"/>
+    <mergeCell ref="F198:F202"/>
+    <mergeCell ref="F203:F207"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A58:B61"/>
@@ -4801,30 +6898,54 @@
     <mergeCell ref="F77:F81"/>
     <mergeCell ref="B83:B84"/>
     <mergeCell ref="F83:F84"/>
+    <mergeCell ref="A240:F240"/>
+    <mergeCell ref="B203:B207"/>
+    <mergeCell ref="B208:B209"/>
+    <mergeCell ref="B210:B211"/>
+    <mergeCell ref="B212:B213"/>
+    <mergeCell ref="B214:B215"/>
+    <mergeCell ref="B216:B219"/>
+    <mergeCell ref="B220:B223"/>
+    <mergeCell ref="B225:B229"/>
+    <mergeCell ref="B230:B235"/>
+    <mergeCell ref="B236:B237"/>
+    <mergeCell ref="B238:B239"/>
+    <mergeCell ref="A151:A239"/>
+    <mergeCell ref="B153:B156"/>
+    <mergeCell ref="B157:B160"/>
+    <mergeCell ref="B161:B164"/>
+    <mergeCell ref="B165:B169"/>
+    <mergeCell ref="F153:F156"/>
+    <mergeCell ref="F157:F160"/>
+    <mergeCell ref="F161:F164"/>
+    <mergeCell ref="B170:B174"/>
+    <mergeCell ref="B175:B178"/>
+    <mergeCell ref="B179:B182"/>
+    <mergeCell ref="B183:B188"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="A5:B10"/>
+    <mergeCell ref="F5:F10"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="F25:F28"/>
+    <mergeCell ref="A29:B31"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="A32:B35"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B43"/>
+    <mergeCell ref="F39:F43"/>
+    <mergeCell ref="A49:B50"/>
+    <mergeCell ref="F49:F50"/>
     <mergeCell ref="A51:B52"/>
     <mergeCell ref="F51:F52"/>
     <mergeCell ref="A53:B55"/>
     <mergeCell ref="F53:F55"/>
     <mergeCell ref="A93:B110"/>
     <mergeCell ref="F93:F110"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B43"/>
-    <mergeCell ref="F39:F43"/>
-    <mergeCell ref="A49:B50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="F25:F28"/>
-    <mergeCell ref="A29:B31"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="A32:B35"/>
-    <mergeCell ref="F32:F35"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="A5:B10"/>
-    <mergeCell ref="F5:F10"/>
-    <mergeCell ref="A113:B123"/>
-    <mergeCell ref="F113:F123"/>
-    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="A111:F112"/>
     <mergeCell ref="A11:B15"/>
     <mergeCell ref="F11:F15"/>
     <mergeCell ref="A16:B17"/>
@@ -4838,6 +6959,30 @@
     <mergeCell ref="A23:B24"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="A25:B28"/>
+    <mergeCell ref="F214:F215"/>
+    <mergeCell ref="F216:F219"/>
+    <mergeCell ref="F220:F223"/>
+    <mergeCell ref="F225:F229"/>
+    <mergeCell ref="F230:F235"/>
+    <mergeCell ref="F236:F237"/>
+    <mergeCell ref="F238:F239"/>
+    <mergeCell ref="B189:B192"/>
+    <mergeCell ref="A113:B123"/>
+    <mergeCell ref="F113:F123"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="F165:F169"/>
+    <mergeCell ref="F170:F174"/>
+    <mergeCell ref="F175:F178"/>
+    <mergeCell ref="F179:F182"/>
+    <mergeCell ref="B193:B197"/>
+    <mergeCell ref="B198:B202"/>
+    <mergeCell ref="A125:B127"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A130:B131"/>
+    <mergeCell ref="F125:F127"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="F183:F188"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C1:C34">

</xml_diff>